<commit_message>
Deploying to gh-pages from @ Healthedata1/USCDI5-Sandbox@396af81b68bc898b944fab795bc9dfa8f67d5ae9 🚀
</commit_message>
<xml_diff>
--- a/CodeSystem-foo-bar.xlsx
+++ b/CodeSystem-foo-bar.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
   <si>
     <t>Property</t>
   </si>
@@ -66,19 +66,22 @@
     <t>Publisher</t>
   </si>
   <si>
-    <t>Health eData Inc</t>
+    <t>HL7 International / Cross-Group Projects</t>
   </si>
   <si>
     <t>Contact</t>
   </si>
   <si>
-    <t>null (mailto:ehaas@healthedatainc.com)</t>
+    <t>HL7 International / Cross-Group Projects (http://www.hl7.org/Special/committees/cgp, cgp@lists.HL7.org)</t>
+  </si>
+  <si>
+    <t>Health eData Inc (mailto:ehaas@healthedatainc.com)</t>
   </si>
   <si>
     <t>Jurisdiction</t>
   </si>
   <si>
-    <t/>
+    <t>United States of America</t>
   </si>
   <si>
     <t>Description</t>
@@ -88,6 +91,9 @@
   </si>
   <si>
     <t>Copyright</t>
+  </si>
+  <si>
+    <t>Used by permission of HL7 International, all rights reserved Creative Commons License</t>
   </si>
   <si>
     <t>Case Sensitive</t>
@@ -275,7 +281,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -367,25 +373,27 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s" s="2">
         <v>20</v>
-      </c>
-      <c r="B11" t="s" s="2">
-        <v>21</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s" s="2">
         <v>22</v>
-      </c>
-      <c r="B12" t="s" s="2">
-        <v>9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" t="s" s="2">
+        <v>9</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
@@ -398,52 +406,60 @@
         <v>25</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>26</v>
-      </c>
-      <c r="B16" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="B16" t="s" s="2">
+        <v>13</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B19" s="2"/>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>30</v>
-      </c>
-      <c r="B20" t="s" s="2">
         <v>31</v>
       </c>
+      <c r="B20" s="2"/>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
         <v>32</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" t="s" s="2">
+        <v>33</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B22" s="2"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="B23" s="2"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -460,44 +476,44 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s" s="1">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>